<commit_message>
Forçando deploy da versão mais recente do carrinho com v3
</commit_message>
<xml_diff>
--- a/Elementos/Produtos.xlsx
+++ b/Elementos/Produtos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oem\Documents\MeuCatalogoOnline\Elementos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3866EC-8C4B-489D-81F3-18C58138EDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6735C6F-441E-419E-B256-1E3639779884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{36164C2F-B5F9-4C19-8D69-FD8539C632E1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
   <si>
     <t>valor</t>
   </si>
@@ -487,7 +487,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +596,175 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forçando deploy da correção final do carrinho
</commit_message>
<xml_diff>
--- a/Elementos/Produtos.xlsx
+++ b/Elementos/Produtos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oem\Documents\MeuCatalogoOnline\Elementos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6735C6F-441E-419E-B256-1E3639779884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274141E5-6F7C-4456-958E-5D23C66EB185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{36164C2F-B5F9-4C19-8D69-FD8539C632E1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>valor</t>
   </si>
@@ -68,9 +68,6 @@
     <t>ofertas</t>
   </si>
   <si>
-    <t>https://i.imgur.com/zanG3Hx.jpg</t>
-  </si>
-  <si>
     <t>https://i.imgur.com/HpwMEIn.jpeg</t>
   </si>
   <si>
@@ -78,6 +75,12 @@
   </si>
   <si>
     <t>https://i.imgur.com/XePLgzW.jpeg</t>
+  </si>
+  <si>
+    <t>Alicate Universal 8" - Promoção</t>
+  </si>
+  <si>
+    <t>Torquês Armador - Promoção</t>
   </si>
 </sst>
 </file>
@@ -481,13 +484,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31746F49-704B-4F8D-8669-71884F6D3547}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +537,7 @@
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -548,7 +551,7 @@
         <v>11.5</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
@@ -562,7 +565,7 @@
         <v>9.5</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>2</v>
@@ -570,7 +573,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4">
         <v>30</v>
@@ -584,188 +587,20 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4">
         <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4">
-        <v>11.5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4">
-        <v>9.5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="4">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="4">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="4">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="4">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="4">
-        <v>11.5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="4">
-        <v>9.5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="4">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="4">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
+      <c r="C11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Forçando o deploy da correção dos produtos de exemplo em carregarProdutosSalvos
</commit_message>
<xml_diff>
--- a/Elementos/Produtos.xlsx
+++ b/Elementos/Produtos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oem\Documents\MeuCatalogoOnline\Elementos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274141E5-6F7C-4456-958E-5D23C66EB185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E676077-C5AD-4CE2-B235-C0D192557EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{36164C2F-B5F9-4C19-8D69-FD8539C632E1}"/>
   </bookViews>
@@ -36,26 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
-  <si>
-    <t>valor</t>
-  </si>
-  <si>
-    <t>menu</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>produtos</t>
   </si>
   <si>
-    <t>imagem_id</t>
-  </si>
-  <si>
-    <t>nome</t>
-  </si>
-  <si>
-    <t>Alicate Universal 8"</t>
-  </si>
-  <si>
     <t>Torquês Armador</t>
   </si>
   <si>
@@ -81,6 +66,45 @@
   </si>
   <si>
     <t>Torquês Armador - Promoção</t>
+  </si>
+  <si>
+    <t>Preco</t>
+  </si>
+  <si>
+    <t>Imagem</t>
+  </si>
+  <si>
+    <t>Prod_1</t>
+  </si>
+  <si>
+    <t>Prod_2</t>
+  </si>
+  <si>
+    <t>Prod_3</t>
+  </si>
+  <si>
+    <t>Prod_4</t>
+  </si>
+  <si>
+    <t>Prod_5</t>
+  </si>
+  <si>
+    <t>Prod_6</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Descricao</t>
+  </si>
+  <si>
+    <t>Menu</t>
   </si>
 </sst>
 </file>
@@ -90,7 +114,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +134,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -149,6 +179,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -484,125 +517,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31746F49-704B-4F8D-8669-71884F6D3547}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>11.5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>9.5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4">
+      <c r="E7" s="4">
         <v>40</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizando URLs das imagens dos produtos
</commit_message>
<xml_diff>
--- a/Elementos/Produtos.xlsx
+++ b/Elementos/Produtos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oem\Documents\MeuCatalogoOnline\Elementos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E676077-C5AD-4CE2-B235-C0D192557EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB2E311-16C1-4900-8476-D019A625AF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{36164C2F-B5F9-4C19-8D69-FD8539C632E1}"/>
   </bookViews>
@@ -523,7 +523,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
       <c r="E3" s="4">
         <v>45</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -603,7 +603,7 @@
       <c r="E4" s="4">
         <v>11.5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -620,7 +620,7 @@
       <c r="E5" s="4">
         <v>9.5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -637,7 +637,7 @@
       <c r="E6" s="4">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -654,7 +654,7 @@
       <c r="E7" s="4">
         <v>40</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -666,6 +666,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{556248C0-1D03-42DF-BDCA-77E5702BA478}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{DE92665B-C0EC-45B4-85EE-B20744B465BB}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{7CEE7C4B-0558-4594-8158-C249D06F8ADD}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{2097AF3C-82B5-4E93-8B4F-D2C11E61BDC2}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{8E317761-D9D8-40DF-ABE2-FB7EF37C8480}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>